<commit_message>
Rubrica 1 terminada :D
</commit_message>
<xml_diff>
--- a/Documentos/Rubrica1/ModeloLogico.xlsx
+++ b/Documentos/Rubrica1/ModeloLogico.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Javier\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ezequiel\Documents\Drive\Proyectos\BDI\BD1Project2019\Documentos\Rubrica1\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90E49B76-8A8C-40FB-92AD-2F12949227BC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28770" windowHeight="12360" tabRatio="647" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="647" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EMPLEADOS" sheetId="30" r:id="rId1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="113">
   <si>
     <t>JUEGO</t>
   </si>
@@ -94,9 +95,6 @@
     <t>LINEA</t>
   </si>
   <si>
-    <t>(Familiar,Institucional</t>
-  </si>
-  <si>
     <t>COLOR</t>
   </si>
   <si>
@@ -340,9 +338,6 @@
     <t>monto_total</t>
   </si>
   <si>
-    <t>factura</t>
-  </si>
-  <si>
     <t>FK_Pedido</t>
   </si>
   <si>
@@ -371,12 +366,15 @@
   </si>
   <si>
     <t>FK5</t>
+  </si>
+  <si>
+    <t>check('F','I')</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -448,7 +446,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -504,15 +502,6 @@
         <color auto="1"/>
       </top>
       <bottom style="thick">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -608,16 +597,31 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -629,14 +633,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -644,52 +642,43 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="33">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Hipervínculo visitado" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -967,32 +956,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H155"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:H156"/>
   <sheetViews>
-    <sheetView topLeftCell="A126" workbookViewId="0">
-      <selection activeCell="D129" sqref="D129"/>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="E84" sqref="E84"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="2" max="3" width="23" customWidth="1"/>
+    <col min="2" max="2" width="36.5703125" customWidth="1"/>
+    <col min="3" max="3" width="23" customWidth="1"/>
     <col min="4" max="4" width="25.42578125" customWidth="1"/>
     <col min="5" max="5" width="25.85546875" customWidth="1"/>
     <col min="6" max="6" width="27.42578125" customWidth="1"/>
-    <col min="7" max="7" width="27.7109375" customWidth="1"/>
+    <col min="7" max="7" width="50.42578125" customWidth="1"/>
     <col min="8" max="8" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="26"/>
+      <c r="A1" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="22"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
@@ -1002,16 +995,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="E2" s="6" t="s">
         <v>57</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>58</v>
       </c>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
@@ -1075,10 +1068,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>5</v>
@@ -1098,35 +1091,35 @@
       <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="18" t="s">
-        <v>53</v>
-      </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-      <c r="D9" s="19"/>
-      <c r="E9" s="19"/>
-      <c r="F9" s="20"/>
+      <c r="A9" s="23" t="s">
+        <v>52</v>
+      </c>
+      <c r="B9" s="25"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="25"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="24"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E10" s="6" t="s">
+      <c r="F10" s="6" t="s">
         <v>71</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>72</v>
       </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
@@ -1153,18 +1146,18 @@
     </row>
     <row r="12" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
@@ -1180,7 +1173,7 @@
         <v>12</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G13" s="2"/>
       <c r="H13" s="1"/>
@@ -1200,10 +1193,10 @@
         <v>5</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>5</v>
@@ -1228,12 +1221,12 @@
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="18" t="s">
-        <v>52</v>
-      </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-      <c r="D17" s="20"/>
+      <c r="A17" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="B17" s="25"/>
+      <c r="C17" s="25"/>
+      <c r="D17" s="24"/>
       <c r="E17" s="2"/>
       <c r="F17" s="1"/>
       <c r="G17" s="2"/>
@@ -1244,13 +1237,13 @@
         <v>1</v>
       </c>
       <c r="B18" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="C18" s="6" t="s">
-        <v>74</v>
-      </c>
       <c r="D18" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E18" s="2"/>
       <c r="F18" s="1"/>
@@ -1277,14 +1270,14 @@
     </row>
     <row r="20" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A20" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" s="6"/>
       <c r="C20" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="1"/>
@@ -1320,7 +1313,7 @@
         <v>5</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>5</v>
@@ -1344,10 +1337,10 @@
       <c r="H24" s="2"/>
     </row>
     <row r="25" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="18" t="s">
-        <v>50</v>
-      </c>
-      <c r="B25" s="20"/>
+      <c r="A25" s="23" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="24"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -1357,10 +1350,10 @@
     </row>
     <row r="26" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -1420,7 +1413,7 @@
         <v>5</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -1440,13 +1433,13 @@
       <c r="H32" s="2"/>
     </row>
     <row r="33" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="B33" s="19"/>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="20"/>
+      <c r="A33" s="23" t="s">
+        <v>47</v>
+      </c>
+      <c r="B33" s="25"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="24"/>
       <c r="F33" s="4"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
@@ -1456,16 +1449,16 @@
         <v>1</v>
       </c>
       <c r="B34" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C34" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="D34" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="D34" s="7" t="s">
+      <c r="E34" s="7" t="s">
         <v>78</v>
-      </c>
-      <c r="E34" s="7" t="s">
-        <v>79</v>
       </c>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
@@ -1521,7 +1514,7 @@
         <v>5</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>5</v>
@@ -1546,11 +1539,11 @@
       <c r="H40" s="2"/>
     </row>
     <row r="41" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="18" t="s">
-        <v>47</v>
-      </c>
-      <c r="B41" s="19"/>
-      <c r="C41" s="20"/>
+      <c r="A41" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B41" s="25"/>
+      <c r="C41" s="24"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
@@ -1562,10 +1555,10 @@
         <v>1</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C42" s="7" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
@@ -1612,7 +1605,7 @@
     <row r="46" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="7"/>
       <c r="B46" s="7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C46" s="7"/>
       <c r="D46" s="2"/>
@@ -1626,10 +1619,10 @@
         <v>5</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
@@ -1648,10 +1641,10 @@
       <c r="H48" s="2"/>
     </row>
     <row r="49" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="18" t="s">
-        <v>46</v>
-      </c>
-      <c r="B49" s="20"/>
+      <c r="A49" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B49" s="24"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
@@ -1664,7 +1657,7 @@
         <v>1</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
@@ -1724,7 +1717,7 @@
         <v>5</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
@@ -1744,10 +1737,10 @@
       <c r="H56" s="2"/>
     </row>
     <row r="57" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="21" t="s">
-        <v>45</v>
-      </c>
-      <c r="B57" s="22"/>
+      <c r="A57" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="B57" s="27"/>
       <c r="C57" s="8"/>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
@@ -1757,10 +1750,10 @@
     </row>
     <row r="58" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
@@ -1783,10 +1776,10 @@
     </row>
     <row r="60" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
@@ -1840,10 +1833,10 @@
       <c r="H64" s="2"/>
     </row>
     <row r="65" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="B65" s="20"/>
+      <c r="A65" s="23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B65" s="24"/>
       <c r="C65" s="4"/>
       <c r="D65" s="3"/>
       <c r="E65" s="3"/>
@@ -1853,10 +1846,10 @@
     </row>
     <row r="66" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B66" s="6" t="s">
         <v>60</v>
-      </c>
-      <c r="B66" s="6" t="s">
-        <v>61</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" s="3"/>
@@ -1881,10 +1874,10 @@
     </row>
     <row r="68" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A68" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" s="3"/>
@@ -1942,41 +1935,41 @@
       <c r="H72" s="2"/>
     </row>
     <row r="73" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="B73" s="23"/>
-      <c r="C73" s="23"/>
-      <c r="D73" s="23"/>
-      <c r="E73" s="23"/>
-      <c r="F73" s="23"/>
-      <c r="G73" s="23"/>
-      <c r="H73" s="23"/>
+      <c r="A73" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="B73" s="28"/>
+      <c r="C73" s="28"/>
+      <c r="D73" s="28"/>
+      <c r="E73" s="28"/>
+      <c r="F73" s="28"/>
+      <c r="G73" s="28"/>
+      <c r="H73" s="28"/>
     </row>
     <row r="74" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D74" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E74" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="E74" s="6" t="s">
+      <c r="F74" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="F74" s="6" t="s">
+      <c r="G74" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="G74" s="6" t="s">
+      <c r="H74" s="6" t="s">
         <v>65</v>
-      </c>
-      <c r="H74" s="6" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2036,10 +2029,10 @@
       <c r="D78" s="6"/>
       <c r="E78" s="6"/>
       <c r="F78" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="G78" s="6" t="s">
         <v>67</v>
-      </c>
-      <c r="G78" s="6" t="s">
-        <v>68</v>
       </c>
       <c r="H78" s="6"/>
     </row>
@@ -2051,40 +2044,38 @@
         <v>5</v>
       </c>
       <c r="C79" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="D79" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="E79" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="F79" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="D79" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="E79" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="F79" s="6" t="s">
-        <v>84</v>
-      </c>
       <c r="G79" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H79" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="80" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="2"/>
-      <c r="B80" s="2"/>
-      <c r="C80" s="2"/>
-      <c r="D80" s="2"/>
-      <c r="E80" s="2"/>
-      <c r="F80" s="2"/>
-      <c r="G80" s="2"/>
-      <c r="H80" s="2"/>
-    </row>
-    <row r="81" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="B81" s="19"/>
-      <c r="C81" s="20"/>
+    <row r="80" spans="1:8" ht="19.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="3"/>
+      <c r="B80" s="3"/>
+      <c r="C80" s="3"/>
+      <c r="D80" s="3"/>
+      <c r="E80" s="3"/>
+      <c r="F80" s="3"/>
+      <c r="G80" s="3"/>
+      <c r="H80" s="3"/>
+    </row>
+    <row r="81" spans="1:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="2"/>
+      <c r="B81" s="2"/>
+      <c r="C81" s="2"/>
       <c r="D81" s="2"/>
       <c r="E81" s="2"/>
       <c r="F81" s="2"/>
@@ -2092,15 +2083,11 @@
       <c r="H81" s="2"/>
     </row>
     <row r="82" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B82" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C82" s="6" t="s">
-        <v>41</v>
-      </c>
+      <c r="A82" s="23" t="s">
+        <v>39</v>
+      </c>
+      <c r="B82" s="25"/>
+      <c r="C82" s="24"/>
       <c r="D82" s="2"/>
       <c r="E82" s="2"/>
       <c r="F82" s="2"/>
@@ -2109,13 +2096,13 @@
     </row>
     <row r="83" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A83" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>3</v>
+        <v>36</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="D83" s="2"/>
       <c r="E83" s="2"/>
@@ -2125,10 +2112,14 @@
     </row>
     <row r="84" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A84" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B84" s="6"/>
-      <c r="C84" s="6"/>
+        <v>3</v>
+      </c>
+      <c r="B84" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C84" s="6" t="s">
+        <v>3</v>
+      </c>
       <c r="D84" s="2"/>
       <c r="E84" s="2"/>
       <c r="F84" s="2"/>
@@ -2136,7 +2127,9 @@
       <c r="H84" s="2"/>
     </row>
     <row r="85" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="6"/>
+      <c r="A85" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="B85" s="6"/>
       <c r="C85" s="6"/>
       <c r="D85" s="2"/>
@@ -2156,153 +2149,156 @@
       <c r="H86" s="2"/>
     </row>
     <row r="87" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B87" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="C87" s="6" t="s">
-        <v>13</v>
-      </c>
+      <c r="A87" s="6"/>
+      <c r="B87" s="6"/>
+      <c r="C87" s="6"/>
       <c r="D87" s="2"/>
       <c r="E87" s="2"/>
       <c r="F87" s="2"/>
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
     </row>
-    <row r="88" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="89" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="18" t="s">
-        <v>88</v>
-      </c>
-      <c r="B89" s="19"/>
-      <c r="C89" s="19"/>
-      <c r="D89" s="20"/>
-    </row>
+    <row r="88" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B88" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C88" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D88" s="2"/>
+      <c r="E88" s="2"/>
+      <c r="F88" s="2"/>
+      <c r="G88" s="2"/>
+      <c r="H88" s="2"/>
+    </row>
+    <row r="89" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="90" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A90" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="B90" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="C90" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D90" s="6" t="s">
-        <v>89</v>
-      </c>
+      <c r="A90" s="23" t="s">
+        <v>87</v>
+      </c>
+      <c r="B90" s="25"/>
+      <c r="C90" s="25"/>
+      <c r="D90" s="24"/>
     </row>
     <row r="91" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A91" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="B91" s="6"/>
+        <v>55</v>
+      </c>
+      <c r="B91" s="6" t="s">
+        <v>56</v>
+      </c>
       <c r="C91" s="6" t="s">
-        <v>3</v>
+        <v>57</v>
       </c>
       <c r="D91" s="6" t="s">
-        <v>3</v>
+        <v>88</v>
       </c>
     </row>
     <row r="92" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A92" s="6" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="B92" s="6"/>
       <c r="C92" s="6" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>25</v>
+        <v>3</v>
       </c>
     </row>
     <row r="93" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="6"/>
+      <c r="A93" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="B93" s="6"/>
       <c r="C93" s="6" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="6"/>
       <c r="B94" s="6"/>
-      <c r="C94" s="6"/>
-      <c r="D94" s="6"/>
+      <c r="C94" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D94" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="95" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B95" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="C95" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D95" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="97" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A97" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="B97" s="19"/>
-      <c r="C97" s="19"/>
-      <c r="D97" s="19"/>
-      <c r="E97" s="20"/>
-    </row>
+      <c r="A95" s="6"/>
+      <c r="B95" s="6"/>
+      <c r="C95" s="6"/>
+      <c r="D95" s="6"/>
+    </row>
+    <row r="96" spans="1:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A96" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B96" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C96" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D96" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="98" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B98" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="C98" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="D98" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="E98" s="6" t="s">
-        <v>94</v>
-      </c>
+      <c r="A98" s="23" t="s">
+        <v>89</v>
+      </c>
+      <c r="B98" s="25"/>
+      <c r="C98" s="25"/>
+      <c r="D98" s="25"/>
+      <c r="E98" s="24"/>
     </row>
     <row r="99" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A99" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>3</v>
+        <v>90</v>
       </c>
       <c r="C99" s="6" t="s">
-        <v>3</v>
+        <v>91</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>3</v>
+        <v>92</v>
       </c>
       <c r="E99" s="6" t="s">
-        <v>3</v>
+        <v>93</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B100" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C100" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D100" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E100" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A101" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B100" s="6"/>
-      <c r="C100" s="6"/>
-      <c r="D100" s="6"/>
-      <c r="E100" s="6"/>
-    </row>
-    <row r="101" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A101" s="6"/>
       <c r="B101" s="6"/>
       <c r="C101" s="6"/>
       <c r="D101" s="6"/>
@@ -2316,208 +2312,211 @@
       <c r="E102" s="6"/>
     </row>
     <row r="103" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B103" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="C103" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D103" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="E103" s="6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="105" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A105" s="18" t="s">
-        <v>95</v>
-      </c>
-      <c r="B105" s="19"/>
-      <c r="C105" s="20"/>
-      <c r="D105" s="4"/>
-    </row>
+      <c r="A103" s="6"/>
+      <c r="B103" s="6"/>
+      <c r="C103" s="6"/>
+      <c r="D103" s="6"/>
+      <c r="E103" s="6"/>
+    </row>
+    <row r="104" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A104" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B104" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C104" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D104" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E104" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="106" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A106" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="B106" s="7" t="s">
-        <v>96</v>
-      </c>
-      <c r="C106" s="7" t="s">
-        <v>78</v>
-      </c>
+      <c r="A106" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="B106" s="25"/>
+      <c r="C106" s="24"/>
+      <c r="D106" s="4"/>
     </row>
     <row r="107" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A107" s="7" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>3</v>
+        <v>77</v>
       </c>
     </row>
     <row r="108" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A108" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B108" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C108" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A109" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B108" s="7"/>
-      <c r="C108" s="7"/>
-    </row>
-    <row r="109" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="7"/>
       <c r="B109" s="7"/>
-      <c r="C109" s="7" t="s">
-        <v>10</v>
-      </c>
+      <c r="C109" s="7"/>
     </row>
     <row r="110" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A110" s="7"/>
       <c r="B110" s="7"/>
-      <c r="C110" s="7"/>
+      <c r="C110" s="7" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="111" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A111" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B111" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C111" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="13"/>
-      <c r="B112" s="13"/>
-      <c r="C112" s="13"/>
-    </row>
-    <row r="113" spans="1:2" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A113" s="18" t="s">
-        <v>97</v>
-      </c>
-      <c r="B113" s="20"/>
-    </row>
-    <row r="114" spans="1:2" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="7" t="s">
+      <c r="A111" s="7"/>
+      <c r="B111" s="7"/>
+      <c r="C111" s="7"/>
+    </row>
+    <row r="112" spans="1:5" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A112" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B112" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C112" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A113" s="13"/>
+      <c r="B113" s="13"/>
+      <c r="C113" s="13"/>
+    </row>
+    <row r="114" spans="1:3" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A114" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="B114" s="24"/>
+    </row>
+    <row r="115" spans="1:3" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A115" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B114" s="7" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="7" t="s">
-        <v>3</v>
-      </c>
       <c r="B115" s="7" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A116" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B116" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A117" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B116" s="7"/>
-    </row>
-    <row r="117" spans="1:2" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A117" s="7"/>
       <c r="B117" s="7"/>
     </row>
-    <row r="118" spans="1:2" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:3" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A118" s="7"/>
       <c r="B118" s="7"/>
     </row>
-    <row r="119" spans="1:2" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A119" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B119" s="7" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="120" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="121" spans="1:2" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A121" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="B121" s="20"/>
-    </row>
-    <row r="122" spans="1:2" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A122" s="6" t="s">
+    <row r="119" spans="1:3" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A119" s="7"/>
+      <c r="B119" s="7"/>
+    </row>
+    <row r="120" spans="1:3" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A120" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B120" s="7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="122" spans="1:3" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A122" s="23" t="s">
+        <v>97</v>
+      </c>
+      <c r="B122" s="24"/>
+    </row>
+    <row r="123" spans="1:3" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A123" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B122" s="6" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A123" s="6" t="s">
-        <v>3</v>
-      </c>
       <c r="B123" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="124" spans="1:3" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B124" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="125" spans="1:3" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B124" s="6"/>
-    </row>
-    <row r="125" spans="1:2" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A125" s="6"/>
       <c r="B125" s="6"/>
     </row>
-    <row r="126" spans="1:2" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:3" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="6"/>
       <c r="B126" s="6"/>
     </row>
-    <row r="127" spans="1:2" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A127" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B127" s="6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="129" spans="1:6" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A129" s="18" t="s">
-        <v>99</v>
-      </c>
-      <c r="B129" s="20"/>
-    </row>
+    <row r="127" spans="1:3" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A127" s="6"/>
+      <c r="B127" s="6"/>
+    </row>
+    <row r="128" spans="1:3" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A128" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B128" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="130" spans="1:6" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A130" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="B130" s="6" t="s">
-        <v>27</v>
-      </c>
+      <c r="A130" s="23" t="s">
+        <v>98</v>
+      </c>
+      <c r="B130" s="24"/>
     </row>
     <row r="131" spans="1:6" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B131" s="6" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
     </row>
     <row r="132" spans="1:6" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B132" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B132" s="6"/>
-    </row>
-    <row r="133" spans="1:6" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A133" s="6"/>
       <c r="B133" s="6"/>
     </row>
     <row r="134" spans="1:6" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2525,101 +2524,63 @@
       <c r="B134" s="6"/>
     </row>
     <row r="135" spans="1:6" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A135" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B135" s="6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="137" spans="1:6" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A137" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="B137" s="19"/>
-      <c r="C137" s="19"/>
-      <c r="D137" s="20"/>
-      <c r="F137" s="15"/>
-    </row>
-    <row r="138" spans="1:6" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A138" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="B138" s="12" t="s">
-        <v>103</v>
-      </c>
-      <c r="C138" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D138" s="12" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A139" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B139" s="12"/>
-      <c r="C139" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="D139" s="12" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="140" spans="1:6" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A140" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="B140" s="12"/>
-      <c r="C140" s="12" t="s">
-        <v>25</v>
-      </c>
-      <c r="D140" s="12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="141" spans="1:6" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A141" s="12"/>
-      <c r="B141" s="12"/>
-      <c r="C141" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="D141" s="12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="142" spans="1:6" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A142" s="12"/>
-      <c r="B142" s="12"/>
-      <c r="C142" s="12"/>
-      <c r="D142" s="12"/>
-    </row>
-    <row r="143" spans="1:6" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A143" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="B143" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C143" s="12" t="s">
-        <v>5</v>
-      </c>
-      <c r="D143" s="12" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="144" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="15"/>
+      <c r="A135" s="6"/>
+      <c r="B135" s="6"/>
+    </row>
+    <row r="136" spans="1:6" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A136" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B136" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="138" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A138" s="4"/>
+      <c r="B138" s="4"/>
+      <c r="C138" s="4"/>
+      <c r="D138" s="4"/>
+      <c r="F138" s="15"/>
+    </row>
+    <row r="139" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A139" s="3"/>
+      <c r="B139" s="3"/>
+      <c r="C139" s="3"/>
+      <c r="D139" s="3"/>
+    </row>
+    <row r="140" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A140" s="3"/>
+      <c r="B140" s="3"/>
+      <c r="C140" s="3"/>
+      <c r="D140" s="3"/>
+    </row>
+    <row r="141" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A141" s="3"/>
+      <c r="B141" s="3"/>
+      <c r="C141" s="3"/>
+      <c r="D141" s="3"/>
+    </row>
+    <row r="142" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A142" s="3"/>
+      <c r="B142" s="3"/>
+      <c r="C142" s="3"/>
+      <c r="D142" s="3"/>
+    </row>
+    <row r="143" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A143" s="3"/>
+      <c r="B143" s="3"/>
+      <c r="C143" s="3"/>
+      <c r="D143" s="3"/>
+    </row>
+    <row r="144" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A144" s="3"/>
+      <c r="B144" s="3"/>
+      <c r="C144" s="3"/>
+      <c r="D144" s="3"/>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="15"/>
-      <c r="B145" s="15"/>
-      <c r="C145" s="15"/>
-      <c r="D145" s="15"/>
-      <c r="E145" s="15"/>
-      <c r="F145" s="15"/>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="15"/>
@@ -2629,15 +2590,33 @@
       <c r="E146" s="15"/>
       <c r="F146" s="15"/>
     </row>
-    <row r="155" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A155" s="17"/>
-      <c r="B155" s="17"/>
-      <c r="C155" s="17"/>
-      <c r="D155" s="16"/>
-      <c r="E155" s="15"/>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A147" s="15"/>
+      <c r="B147" s="15"/>
+      <c r="C147" s="15"/>
+      <c r="D147" s="15"/>
+      <c r="E147" s="15"/>
+      <c r="F147" s="15"/>
+    </row>
+    <row r="156" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A156" s="19"/>
+      <c r="B156" s="19"/>
+      <c r="C156" s="19"/>
+      <c r="D156" s="16"/>
+      <c r="E156" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="17">
+    <mergeCell ref="A122:B122"/>
+    <mergeCell ref="A130:B130"/>
+    <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A90:D90"/>
+    <mergeCell ref="A98:E98"/>
+    <mergeCell ref="A114:B114"/>
+    <mergeCell ref="A73:H73"/>
+    <mergeCell ref="A82:C82"/>
+    <mergeCell ref="A106:C106"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A49:B49"/>
     <mergeCell ref="A9:F9"/>
@@ -2645,21 +2624,9 @@
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="A33:E33"/>
     <mergeCell ref="A41:C41"/>
-    <mergeCell ref="A57:B57"/>
-    <mergeCell ref="A89:D89"/>
-    <mergeCell ref="A97:E97"/>
-    <mergeCell ref="A113:B113"/>
-    <mergeCell ref="A73:H73"/>
-    <mergeCell ref="A81:C81"/>
-    <mergeCell ref="A105:C105"/>
-    <mergeCell ref="A155:C155"/>
-    <mergeCell ref="A137:D137"/>
-    <mergeCell ref="A121:B121"/>
-    <mergeCell ref="A129:B129"/>
-    <mergeCell ref="A65:B65"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="43" fitToHeight="0" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2669,14 +2636,17 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:O88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A60" workbookViewId="0">
-      <selection activeCell="E61" sqref="E61"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="22.85546875" customWidth="1"/>
     <col min="3" max="3" width="23" customWidth="1"/>
@@ -2688,11 +2658,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
@@ -2703,10 +2673,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C2" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
@@ -2765,7 +2735,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
@@ -2782,34 +2752,34 @@
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="23" t="s">
-        <v>59</v>
-      </c>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="23"/>
+      <c r="A9" s="28" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
       <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>87</v>
-      </c>
-      <c r="D10" s="6" t="s">
+      <c r="E10" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="F10" s="6" t="s">
         <v>29</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>30</v>
       </c>
       <c r="G10" s="2"/>
     </row>
@@ -2834,15 +2804,15 @@
     </row>
     <row r="12" spans="1:7" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F12" s="6"/>
       <c r="G12" s="2"/>
@@ -2871,7 +2841,7 @@
     </row>
     <row r="15" spans="1:7" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>5</v>
@@ -2880,13 +2850,13 @@
         <v>5</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>5</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G15" s="2"/>
     </row>
@@ -2900,11 +2870,11 @@
       <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="23" t="s">
-        <v>26</v>
-      </c>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
+      <c r="A17" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
@@ -2974,10 +2944,10 @@
         <v>5</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C23" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -2994,11 +2964,11 @@
       <c r="G24" s="2"/>
     </row>
     <row r="25" spans="1:7" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B25" s="23"/>
-      <c r="C25" s="23"/>
+      <c r="A25" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" s="28"/>
+      <c r="C25" s="28"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
@@ -3012,7 +2982,7 @@
         <v>9</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -3036,13 +3006,13 @@
     </row>
     <row r="28" spans="1:7" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -3096,10 +3066,10 @@
       <c r="G32" s="2"/>
     </row>
     <row r="33" spans="1:7" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="23" t="s">
-        <v>22</v>
-      </c>
-      <c r="B33" s="23"/>
+      <c r="A33" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" s="28"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -3166,7 +3136,7 @@
         <v>5</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
@@ -3184,11 +3154,11 @@
       <c r="G40" s="2"/>
     </row>
     <row r="41" spans="1:7" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="23" t="s">
+      <c r="A41" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="B41" s="23"/>
-      <c r="C41" s="23"/>
+      <c r="B41" s="28"/>
+      <c r="C41" s="28"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
@@ -3244,10 +3214,10 @@
       <c r="F45" s="2"/>
       <c r="G45" s="2"/>
     </row>
-    <row r="46" spans="1:7" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="11"/>
       <c r="B46" s="11" t="s">
-        <v>21</v>
+        <v>112</v>
       </c>
       <c r="C46" s="11"/>
       <c r="D46" s="2"/>
@@ -3260,10 +3230,10 @@
         <v>5</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
@@ -3280,12 +3250,12 @@
       <c r="G48" s="2"/>
     </row>
     <row r="49" spans="1:15" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="23" t="s">
+      <c r="A49" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B49" s="23"/>
-      <c r="C49" s="23"/>
-      <c r="D49" s="23"/>
+      <c r="B49" s="28"/>
+      <c r="C49" s="28"/>
+      <c r="D49" s="28"/>
       <c r="E49" s="2"/>
       <c r="F49" s="2"/>
       <c r="G49" s="2"/>
@@ -3360,10 +3330,10 @@
         <v>5</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D55" s="11" t="s">
         <v>5</v>
@@ -3382,11 +3352,11 @@
       <c r="G56" s="2"/>
     </row>
     <row r="57" spans="1:15" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="27" t="s">
+      <c r="A57" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="B57" s="27"/>
-      <c r="C57" s="27"/>
+      <c r="B57" s="30"/>
+      <c r="C57" s="30"/>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
       <c r="F57" s="2"/>
@@ -3466,7 +3436,7 @@
         <v>5</v>
       </c>
       <c r="B63" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C63" s="11" t="s">
         <v>5</v>
@@ -3502,17 +3472,17 @@
       <c r="O64" s="1"/>
     </row>
     <row r="65" spans="1:15" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A65" s="27" t="s">
+      <c r="A65" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B65" s="27"/>
-      <c r="C65" s="27"/>
-      <c r="D65" s="27"/>
-      <c r="E65" s="27"/>
-      <c r="F65" s="27"/>
-      <c r="G65" s="27"/>
-      <c r="H65" s="27"/>
-      <c r="I65" s="27"/>
+      <c r="B65" s="30"/>
+      <c r="C65" s="30"/>
+      <c r="D65" s="30"/>
+      <c r="E65" s="30"/>
+      <c r="F65" s="30"/>
+      <c r="G65" s="30"/>
+      <c r="H65" s="30"/>
+      <c r="I65" s="30"/>
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
       <c r="L65" s="1"/>
@@ -3534,19 +3504,19 @@
         <v>7</v>
       </c>
       <c r="E66" s="11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F66" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G66" s="11" t="s">
         <v>9</v>
       </c>
       <c r="H66" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="I66" s="14" t="s">
         <v>110</v>
-      </c>
-      <c r="I66" s="14" t="s">
-        <v>112</v>
       </c>
       <c r="J66" s="1"/>
       <c r="K66" s="1"/>
@@ -3617,13 +3587,13 @@
         <v>12</v>
       </c>
       <c r="G69" s="11" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H69" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="I69" s="14" t="s">
         <v>111</v>
-      </c>
-      <c r="I69" s="14" t="s">
-        <v>113</v>
       </c>
       <c r="J69" s="1"/>
       <c r="K69" s="1"/>
@@ -3657,10 +3627,10 @@
         <v>13</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D71" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E71" s="11" t="s">
         <v>5</v>
@@ -3695,10 +3665,10 @@
       <c r="O72" s="1"/>
     </row>
     <row r="73" spans="1:15" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A73" s="32" t="s">
-        <v>106</v>
-      </c>
-      <c r="B73" s="32"/>
+      <c r="A73" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="B73" s="29"/>
       <c r="H73" s="1"/>
       <c r="I73" s="1"/>
       <c r="J73" s="1"/>
@@ -3709,10 +3679,10 @@
       <c r="O73" s="1"/>
     </row>
     <row r="74" spans="1:15" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A74" s="31" t="s">
+      <c r="A74" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B74" s="31" t="s">
+      <c r="B74" s="18" t="s">
         <v>2</v>
       </c>
       <c r="H74" s="1"/>
@@ -3725,10 +3695,10 @@
       <c r="O74" s="1"/>
     </row>
     <row r="75" spans="1:15" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A75" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="B75" s="31" t="s">
+      <c r="A75" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B75" s="18" t="s">
         <v>3</v>
       </c>
       <c r="H75" s="1"/>
@@ -3741,89 +3711,89 @@
       <c r="O75" s="1"/>
     </row>
     <row r="76" spans="1:15" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A76" s="31" t="s">
+      <c r="A76" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B76" s="31"/>
+      <c r="B76" s="18"/>
     </row>
     <row r="77" spans="1:15" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A77" s="31"/>
-      <c r="B77" s="31"/>
+      <c r="A77" s="18"/>
+      <c r="B77" s="18"/>
     </row>
     <row r="78" spans="1:15" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A78" s="31"/>
-      <c r="B78" s="31"/>
+      <c r="A78" s="18"/>
+      <c r="B78" s="18"/>
     </row>
     <row r="79" spans="1:15" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A79" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="B79" s="31" t="s">
-        <v>81</v>
+      <c r="A79" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B79" s="18" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="80" spans="1:15" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="81" spans="1:2" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A81" s="32" t="s">
-        <v>109</v>
-      </c>
-      <c r="B81" s="32"/>
+      <c r="A81" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="B81" s="29"/>
     </row>
     <row r="82" spans="1:2" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A82" s="31" t="s">
+      <c r="A82" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B82" s="31" t="s">
+      <c r="B82" s="18" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A83" s="31" t="s">
-        <v>3</v>
-      </c>
-      <c r="B83" s="31" t="s">
+      <c r="A83" s="18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B83" s="18" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A84" s="31" t="s">
+      <c r="A84" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="B84" s="31"/>
+      <c r="B84" s="18"/>
     </row>
     <row r="85" spans="1:2" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A85" s="31"/>
-      <c r="B85" s="31"/>
+      <c r="A85" s="18"/>
+      <c r="B85" s="18"/>
     </row>
     <row r="86" spans="1:2" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A86" s="31"/>
-      <c r="B86" s="31"/>
+      <c r="A86" s="18"/>
+      <c r="B86" s="18"/>
     </row>
     <row r="87" spans="1:2" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A87" s="31" t="s">
-        <v>5</v>
-      </c>
-      <c r="B87" s="31" t="s">
-        <v>81</v>
+      <c r="A87" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B87" s="18" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="11">
+    <mergeCell ref="A41:C41"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A9:F9"/>
+    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A25:C25"/>
+    <mergeCell ref="A33:B33"/>
     <mergeCell ref="A73:B73"/>
     <mergeCell ref="A81:B81"/>
     <mergeCell ref="A65:I65"/>
     <mergeCell ref="A49:D49"/>
     <mergeCell ref="A57:C57"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A9:F9"/>
-    <mergeCell ref="A17:C17"/>
-    <mergeCell ref="A25:C25"/>
-    <mergeCell ref="A33:B33"/>
-    <mergeCell ref="A41:C41"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="40" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3833,14 +3803,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
   <dimension ref="A1:D40"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.28515625" customWidth="1"/>
     <col min="2" max="2" width="24.28515625" customWidth="1"/>
@@ -3849,10 +3822,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="23" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="23"/>
+      <c r="A1" s="28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="28"/>
       <c r="C1" s="2"/>
     </row>
     <row r="2" spans="1:3" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -3860,7 +3833,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="2"/>
     </row>
@@ -3895,7 +3868,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C7" s="2"/>
     </row>
@@ -3905,18 +3878,18 @@
       <c r="C8" s="2"/>
     </row>
     <row r="9" spans="1:3" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="23" t="s">
-        <v>33</v>
-      </c>
-      <c r="B9" s="23"/>
+      <c r="A9" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="28"/>
       <c r="C9" s="2"/>
     </row>
     <row r="10" spans="1:3" ht="39" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="11" t="s">
         <v>34</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>35</v>
       </c>
       <c r="C10" s="2"/>
     </row>
@@ -3948,10 +3921,10 @@
     </row>
     <row r="15" spans="1:3" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" s="2"/>
     </row>
@@ -3961,25 +3934,25 @@
       <c r="C16" s="2"/>
     </row>
     <row r="17" spans="1:4" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="23" t="s">
-        <v>39</v>
-      </c>
-      <c r="B17" s="23"/>
-      <c r="C17" s="23"/>
-      <c r="D17" s="23"/>
+      <c r="A17" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
     </row>
     <row r="18" spans="1:4" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B18" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C18" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="D18" s="11" t="s">
         <v>102</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4023,13 +3996,13 @@
         <v>5</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4038,18 +4011,18 @@
       <c r="C24" s="2"/>
     </row>
     <row r="25" spans="1:4" ht="38.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="B25" s="30"/>
+      <c r="A25" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="32"/>
       <c r="C25" s="2"/>
     </row>
     <row r="26" spans="1:4" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="29" t="s">
-        <v>27</v>
-      </c>
-      <c r="B26" s="29" t="s">
-        <v>105</v>
+      <c r="A26" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="17" t="s">
+        <v>103</v>
       </c>
       <c r="C26" s="2"/>
     </row>
@@ -4081,10 +4054,10 @@
     </row>
     <row r="31" spans="1:4" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C31" s="2"/>
     </row>
@@ -4094,10 +4067,10 @@
       <c r="C32" s="2"/>
     </row>
     <row r="33" spans="1:3" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="B33" s="23"/>
+      <c r="A33" s="28" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33" s="28"/>
       <c r="C33" s="2"/>
     </row>
     <row r="34" spans="1:3" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -4105,7 +4078,7 @@
         <v>1</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C34" s="2"/>
     </row>
@@ -4140,7 +4113,7 @@
         <v>5</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C39" s="2"/>
     </row>
@@ -4153,8 +4126,8 @@
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="A17:D17"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="86" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>